<commit_message>
Adding result classes to the image importer
</commit_message>
<xml_diff>
--- a/Documentation/ImageImportParameters.xlsx
+++ b/Documentation/ImageImportParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morten Lang\source\repos\SudokuSolver\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812A73C7-C07D-4FC2-8C3D-898960BA849F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AACCC80-9A7B-49B4-B85D-70D866E252E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25380" yWindow="2535" windowWidth="22560" windowHeight="15345" xr2:uid="{5FE21BC2-CD55-4BFA-BB0D-AC0D8CDED28F}"/>
+    <workbookView xWindow="9180" yWindow="2790" windowWidth="19050" windowHeight="11790" xr2:uid="{5FE21BC2-CD55-4BFA-BB0D-AC0D8CDED28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Filename</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>1 false positive + handwritten numbers</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -193,10 +199,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554AAAE3-BCA1-49C5-B74B-2DE704DC3AAC}">
-  <dimension ref="B1:K20"/>
+  <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,27 +550,28 @@
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="9" width="12.140625" customWidth="1"/>
+    <col min="8" max="10" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -590,13 +597,16 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -610,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -629,11 +639,14 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -647,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -666,11 +679,14 @@
       <c r="H6">
         <v>2</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -689,11 +705,14 @@
       <c r="H7">
         <v>2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -707,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -726,14 +745,17 @@
       <c r="H9">
         <v>3</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
         <v>29</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -747,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -761,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -780,11 +802,14 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -798,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -817,14 +842,17 @@
       <c r="H14">
         <v>5</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
         <v>29</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -837,11 +865,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -864,13 +892,16 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" t="s">
         <v>33</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -883,20 +914,23 @@
       <c r="F17">
         <v>7</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" t="s">
         <v>29</v>
       </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -916,10 +950,13 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -932,11 +969,11 @@
       <c r="F19">
         <v>5</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>36</v>
       </c>
@@ -949,7 +986,7 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>